<commit_message>
Corrections to Aditi's list
</commit_message>
<xml_diff>
--- a/D-242 Wine Institute list.xlsx
+++ b/D-242 Wine Institute list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Departments\Cataloging\Students\Aditi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecphillips\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="8685"/>
   </bookViews>
   <sheets>
     <sheet name="Publications" sheetId="1" r:id="rId1"/>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B301" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E333" sqref="E333"/>
+    <sheetView tabSelected="1" topLeftCell="A310" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6510,6 +6510,9 @@
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A324" s="1">
+        <v>164</v>
+      </c>
       <c r="B324" s="2">
         <v>89</v>
       </c>
@@ -6524,8 +6527,11 @@
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A325" s="1">
+        <v>164</v>
+      </c>
       <c r="B325" s="2">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C325" t="s">
         <v>191</v>
@@ -6538,8 +6544,11 @@
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A326" s="1">
+        <v>164</v>
+      </c>
       <c r="B326" s="2">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="C326" t="s">
         <v>191</v>
@@ -6552,8 +6561,11 @@
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A327" s="1">
+        <v>164</v>
+      </c>
       <c r="B327" s="2">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="C327" t="s">
         <v>191</v>
@@ -6566,8 +6578,11 @@
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A328" s="1">
+        <v>164</v>
+      </c>
       <c r="B328" s="2">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="C328" t="s">
         <v>191</v>
@@ -6580,8 +6595,11 @@
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A329" s="1">
+        <v>164</v>
+      </c>
       <c r="B329" s="2">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="C329" t="s">
         <v>191</v>
@@ -6594,8 +6612,11 @@
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A330" s="1">
+        <v>164</v>
+      </c>
       <c r="B330" s="2">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="C330" t="s">
         <v>191</v>
@@ -6608,8 +6629,11 @@
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A331" s="1">
+        <v>164</v>
+      </c>
       <c r="B331" s="2">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="C331" t="s">
         <v>191</v>
@@ -6622,8 +6646,11 @@
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A332" s="1">
+        <v>164</v>
+      </c>
       <c r="B332" s="2">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C332" t="s">
         <v>191</v>
@@ -6636,8 +6663,11 @@
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A333" s="1">
+        <v>164</v>
+      </c>
       <c r="B333" s="2">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="C333" t="s">
         <v>205</v>

</xml_diff>

<commit_message>
Backfilling boxes 156 and 164
</commit_message>
<xml_diff>
--- a/D-242 Wine Institute list.xlsx
+++ b/D-242 Wine Institute list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="232">
   <si>
     <t>Date</t>
   </si>
@@ -533,9 +533,6 @@
     <t>Volume 3: issue 51 (4 copies), 52 (4 copies),53 (4 copies), 54 (4 copies), 56 (5 copies), 58 (3 copies), 59 (4 copies), 60  (3 copies)</t>
   </si>
   <si>
-    <t>Impact</t>
-  </si>
-  <si>
     <t>index 1988</t>
   </si>
   <si>
@@ -672,6 +669,57 @@
   </si>
   <si>
     <t>Volume XII: Number 5</t>
+  </si>
+  <si>
+    <t>OIV General Assembly Resolutions</t>
+  </si>
+  <si>
+    <t>73rd General Assembly, San Francisco</t>
+  </si>
+  <si>
+    <t>American Wine &amp; Food</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>Volume 3, numbers 2-7,9</t>
+  </si>
+  <si>
+    <t>Needs Assessment: Sonoma State University's School of Business &amp; Economics - Wine Business Education Program</t>
+  </si>
+  <si>
+    <t>January 1996</t>
+  </si>
+  <si>
+    <t>Impact Report</t>
+  </si>
+  <si>
+    <t>"Wineries of the Napa Valley" brochure and map</t>
+  </si>
+  <si>
+    <t>Napa Valley Vintner's Association; Napa Valley Grape Growers Association</t>
+  </si>
+  <si>
+    <t>Compass Maps Winery Guide to Northern and Central California</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>"Wine and Public Opinion", Howard Goldberg</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>Photocopy from The Journal of Gastronomy</t>
+  </si>
+  <si>
+    <t>Newsletter of the Americas (International Wine and Food Society)</t>
+  </si>
+  <si>
+    <t>Number 3/1991</t>
   </si>
 </sst>
 </file>
@@ -707,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -720,6 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F333"/>
+  <dimension ref="A1:F340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C333" sqref="C333"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A240" sqref="A240:XFD242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4715,13 +4764,13 @@
         <v>93</v>
       </c>
       <c r="C218" t="s">
+        <v>222</v>
+      </c>
+      <c r="D218" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D218" s="3" t="s">
+      <c r="E218" t="s">
         <v>170</v>
-      </c>
-      <c r="E218" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -4732,10 +4781,10 @@
         <v>94</v>
       </c>
       <c r="C219" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D219" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E219" t="s">
         <v>71</v>
@@ -4749,7 +4798,7 @@
         <v>95</v>
       </c>
       <c r="C220" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D220" s="3">
         <v>32143</v>
@@ -4766,7 +4815,7 @@
         <v>96</v>
       </c>
       <c r="C221" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D221" s="3">
         <v>32174</v>
@@ -4783,7 +4832,7 @@
         <v>97</v>
       </c>
       <c r="C222" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D222" s="3">
         <v>32203</v>
@@ -4800,7 +4849,7 @@
         <v>98</v>
       </c>
       <c r="C223" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D223" s="3">
         <v>32234</v>
@@ -4817,7 +4866,7 @@
         <v>99</v>
       </c>
       <c r="C224" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D224" s="3">
         <v>32264</v>
@@ -4834,7 +4883,7 @@
         <v>100</v>
       </c>
       <c r="C225" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D225" s="3">
         <v>32325</v>
@@ -4851,7 +4900,7 @@
         <v>101</v>
       </c>
       <c r="C226" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D226" s="3">
         <v>32356</v>
@@ -4868,10 +4917,10 @@
         <v>102</v>
       </c>
       <c r="C227" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D227" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E227" t="s">
         <v>71</v>
@@ -4885,7 +4934,7 @@
         <v>103</v>
       </c>
       <c r="C228" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D228" s="3">
         <v>32387</v>
@@ -4902,7 +4951,7 @@
         <v>104</v>
       </c>
       <c r="C229" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D229" s="3">
         <v>32417</v>
@@ -4919,7 +4968,7 @@
         <v>105</v>
       </c>
       <c r="C230" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D230" s="3">
         <v>32448</v>
@@ -4936,7 +4985,7 @@
         <v>106</v>
       </c>
       <c r="C231" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D231" s="3">
         <v>32478</v>
@@ -4953,10 +5002,10 @@
         <v>107</v>
       </c>
       <c r="C232" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E232" t="s">
         <v>71</v>
@@ -4970,7 +5019,7 @@
         <v>108</v>
       </c>
       <c r="C233" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D233" s="3">
         <v>32509</v>
@@ -4987,7 +5036,7 @@
         <v>109</v>
       </c>
       <c r="C234" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D234" s="3">
         <v>32540</v>
@@ -5004,7 +5053,7 @@
         <v>110</v>
       </c>
       <c r="C235" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D235" s="3">
         <v>32599</v>
@@ -5015,70 +5064,67 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B236" s="2">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="C236" t="s">
-        <v>169</v>
-      </c>
-      <c r="D236" s="3">
-        <v>32629</v>
+        <v>223</v>
+      </c>
+      <c r="D236" s="6">
+        <v>1988</v>
       </c>
       <c r="E236" t="s">
-        <v>176</v>
+        <v>224</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B237" s="2">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="C237" t="s">
-        <v>169</v>
-      </c>
-      <c r="D237" s="3">
-        <v>32660</v>
-      </c>
-      <c r="E237" t="s">
-        <v>71</v>
+        <v>225</v>
+      </c>
+      <c r="D237" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B238" s="2">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="C238" t="s">
-        <v>169</v>
-      </c>
-      <c r="D238" t="s">
-        <v>177</v>
+        <v>227</v>
+      </c>
+      <c r="D238" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="E238" t="s">
-        <v>71</v>
+        <v>229</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B239" s="2">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="C239" t="s">
-        <v>169</v>
-      </c>
-      <c r="D239" s="3">
-        <v>32690</v>
+        <v>230</v>
+      </c>
+      <c r="D239" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="E239" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -5086,16 +5132,16 @@
         <v>164</v>
       </c>
       <c r="B240" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C240" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D240" s="3">
-        <v>32721</v>
+        <v>32629</v>
       </c>
       <c r="E240" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -5103,13 +5149,13 @@
         <v>164</v>
       </c>
       <c r="B241" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C241" t="s">
-        <v>169</v>
-      </c>
-      <c r="D241" t="s">
-        <v>175</v>
+        <v>222</v>
+      </c>
+      <c r="D241" s="3">
+        <v>32660</v>
       </c>
       <c r="E241" t="s">
         <v>71</v>
@@ -5120,13 +5166,13 @@
         <v>164</v>
       </c>
       <c r="B242" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C242" t="s">
-        <v>169</v>
-      </c>
-      <c r="D242" s="3">
-        <v>32752</v>
+        <v>222</v>
+      </c>
+      <c r="D242" t="s">
+        <v>176</v>
       </c>
       <c r="E242" t="s">
         <v>71</v>
@@ -5137,16 +5183,16 @@
         <v>164</v>
       </c>
       <c r="B243" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C243" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D243" s="3">
-        <v>32782</v>
+        <v>32690</v>
       </c>
       <c r="E243" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -5154,16 +5200,16 @@
         <v>164</v>
       </c>
       <c r="B244" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C244" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D244" s="3">
-        <v>32813</v>
+        <v>32721</v>
       </c>
       <c r="E244" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -5171,13 +5217,13 @@
         <v>164</v>
       </c>
       <c r="B245" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C245" t="s">
-        <v>169</v>
-      </c>
-      <c r="D245" s="3">
-        <v>32843</v>
+        <v>222</v>
+      </c>
+      <c r="D245" t="s">
+        <v>174</v>
       </c>
       <c r="E245" t="s">
         <v>71</v>
@@ -5188,13 +5234,13 @@
         <v>164</v>
       </c>
       <c r="B246" s="2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C246" t="s">
-        <v>169</v>
-      </c>
-      <c r="D246" t="s">
-        <v>179</v>
+        <v>222</v>
+      </c>
+      <c r="D246" s="3">
+        <v>32752</v>
       </c>
       <c r="E246" t="s">
         <v>71</v>
@@ -5205,16 +5251,16 @@
         <v>164</v>
       </c>
       <c r="B247" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C247" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D247" s="3">
-        <v>32874</v>
+        <v>32782</v>
       </c>
       <c r="E247" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -5222,16 +5268,16 @@
         <v>164</v>
       </c>
       <c r="B248" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C248" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D248" s="3">
-        <v>32905</v>
+        <v>32813</v>
       </c>
       <c r="E248" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -5239,13 +5285,13 @@
         <v>164</v>
       </c>
       <c r="B249" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C249" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D249" s="3">
-        <v>32933</v>
+        <v>32843</v>
       </c>
       <c r="E249" t="s">
         <v>71</v>
@@ -5256,13 +5302,13 @@
         <v>164</v>
       </c>
       <c r="B250" s="2">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C250" t="s">
-        <v>169</v>
-      </c>
-      <c r="D250" s="3">
-        <v>32964</v>
+        <v>222</v>
+      </c>
+      <c r="D250" t="s">
+        <v>178</v>
       </c>
       <c r="E250" t="s">
         <v>71</v>
@@ -5273,13 +5319,13 @@
         <v>164</v>
       </c>
       <c r="B251" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C251" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D251" s="3">
-        <v>32994</v>
+        <v>32874</v>
       </c>
       <c r="E251" t="s">
         <v>71</v>
@@ -5290,16 +5336,16 @@
         <v>164</v>
       </c>
       <c r="B252" s="2">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C252" t="s">
-        <v>169</v>
-      </c>
-      <c r="D252" t="s">
-        <v>178</v>
+        <v>222</v>
+      </c>
+      <c r="D252" s="3">
+        <v>32905</v>
       </c>
       <c r="E252" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -5307,13 +5353,13 @@
         <v>164</v>
       </c>
       <c r="B253" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C253" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D253" s="3">
-        <v>33025</v>
+        <v>32933</v>
       </c>
       <c r="E253" t="s">
         <v>71</v>
@@ -5324,16 +5370,16 @@
         <v>164</v>
       </c>
       <c r="B254" s="2">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C254" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D254" s="3">
-        <v>33055</v>
+        <v>32964</v>
       </c>
       <c r="E254" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -5341,13 +5387,13 @@
         <v>164</v>
       </c>
       <c r="B255" s="2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C255" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D255" s="3">
-        <v>33117</v>
+        <v>32994</v>
       </c>
       <c r="E255" t="s">
         <v>71</v>
@@ -5358,13 +5404,13 @@
         <v>164</v>
       </c>
       <c r="B256" s="2">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C256" t="s">
-        <v>169</v>
-      </c>
-      <c r="D256" s="3">
-        <v>33147</v>
+        <v>222</v>
+      </c>
+      <c r="D256" t="s">
+        <v>177</v>
       </c>
       <c r="E256" t="s">
         <v>75</v>
@@ -5375,16 +5421,16 @@
         <v>164</v>
       </c>
       <c r="B257" s="2">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C257" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D257" s="3">
-        <v>33178</v>
+        <v>33025</v>
       </c>
       <c r="E257" t="s">
-        <v>180</v>
+        <v>71</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -5392,16 +5438,16 @@
         <v>164</v>
       </c>
       <c r="B258" s="2">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C258" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D258" s="3">
-        <v>33208</v>
+        <v>33055</v>
       </c>
       <c r="E258" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -5409,13 +5455,13 @@
         <v>164</v>
       </c>
       <c r="B259" s="2">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C259" t="s">
-        <v>169</v>
-      </c>
-      <c r="D259" s="3" t="s">
-        <v>181</v>
+        <v>222</v>
+      </c>
+      <c r="D259" s="3">
+        <v>33117</v>
       </c>
       <c r="E259" t="s">
         <v>71</v>
@@ -5426,16 +5472,16 @@
         <v>164</v>
       </c>
       <c r="B260" s="2">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C260" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D260" s="3">
-        <v>33239</v>
+        <v>33147</v>
       </c>
       <c r="E260" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -5443,16 +5489,16 @@
         <v>164</v>
       </c>
       <c r="B261" s="2">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C261" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D261" s="3">
-        <v>33270</v>
+        <v>33178</v>
       </c>
       <c r="E261" t="s">
-        <v>71</v>
+        <v>179</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -5460,16 +5506,16 @@
         <v>164</v>
       </c>
       <c r="B262" s="2">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C262" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D262" s="3">
-        <v>33298</v>
+        <v>33208</v>
       </c>
       <c r="E262" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -5477,13 +5523,13 @@
         <v>164</v>
       </c>
       <c r="B263" s="2">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C263" t="s">
-        <v>169</v>
-      </c>
-      <c r="D263" s="3">
-        <v>33329</v>
+        <v>222</v>
+      </c>
+      <c r="D263" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="E263" t="s">
         <v>71</v>
@@ -5494,13 +5540,13 @@
         <v>164</v>
       </c>
       <c r="B264" s="2">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C264" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D264" s="3">
-        <v>33359</v>
+        <v>33239</v>
       </c>
       <c r="E264" t="s">
         <v>71</v>
@@ -5511,13 +5557,13 @@
         <v>164</v>
       </c>
       <c r="B265" s="2">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C265" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D265" s="3">
-        <v>33420</v>
+        <v>33270</v>
       </c>
       <c r="E265" t="s">
         <v>71</v>
@@ -5528,16 +5574,16 @@
         <v>164</v>
       </c>
       <c r="B266" s="2">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C266" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D266" s="3">
-        <v>33482</v>
+        <v>33298</v>
       </c>
       <c r="E266" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -5545,13 +5591,13 @@
         <v>164</v>
       </c>
       <c r="B267" s="2">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C267" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D267" s="3">
-        <v>33543</v>
+        <v>33329</v>
       </c>
       <c r="E267" t="s">
         <v>71</v>
@@ -5562,13 +5608,13 @@
         <v>164</v>
       </c>
       <c r="B268" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C268" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D268" s="3">
-        <v>33573</v>
+        <v>33359</v>
       </c>
       <c r="E268" t="s">
         <v>71</v>
@@ -5579,16 +5625,16 @@
         <v>164</v>
       </c>
       <c r="B269" s="2">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C269" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D269" s="3">
-        <v>33604</v>
+        <v>33420</v>
       </c>
       <c r="E269" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -5596,16 +5642,16 @@
         <v>164</v>
       </c>
       <c r="B270" s="2">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C270" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D270" s="3">
-        <v>33635</v>
+        <v>33482</v>
       </c>
       <c r="E270" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -5613,13 +5659,13 @@
         <v>164</v>
       </c>
       <c r="B271" s="2">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C271" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D271" s="3">
-        <v>33664</v>
+        <v>33543</v>
       </c>
       <c r="E271" t="s">
         <v>71</v>
@@ -5630,13 +5676,13 @@
         <v>164</v>
       </c>
       <c r="B272" s="2">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C272" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D272" s="3">
-        <v>33756</v>
+        <v>33573</v>
       </c>
       <c r="E272" t="s">
         <v>71</v>
@@ -5647,16 +5693,16 @@
         <v>164</v>
       </c>
       <c r="B273" s="2">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C273" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D273" s="3">
-        <v>33786</v>
+        <v>33604</v>
       </c>
       <c r="E273" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -5664,16 +5710,16 @@
         <v>164</v>
       </c>
       <c r="B274" s="2">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C274" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D274" s="3">
-        <v>33817</v>
+        <v>33635</v>
       </c>
       <c r="E274" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -5681,13 +5727,13 @@
         <v>164</v>
       </c>
       <c r="B275" s="2">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C275" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D275" s="3">
-        <v>33848</v>
+        <v>33664</v>
       </c>
       <c r="E275" t="s">
         <v>71</v>
@@ -5698,13 +5744,13 @@
         <v>164</v>
       </c>
       <c r="B276" s="2">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C276" t="s">
-        <v>169</v>
-      </c>
-      <c r="D276" t="s">
-        <v>182</v>
+        <v>222</v>
+      </c>
+      <c r="D276" s="3">
+        <v>33756</v>
       </c>
       <c r="E276" t="s">
         <v>71</v>
@@ -5715,13 +5761,13 @@
         <v>164</v>
       </c>
       <c r="B277" s="2">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C277" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D277" s="3">
-        <v>33878</v>
+        <v>33786</v>
       </c>
       <c r="E277" t="s">
         <v>71</v>
@@ -5732,13 +5778,13 @@
         <v>164</v>
       </c>
       <c r="B278" s="2">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C278" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D278" s="3">
-        <v>34274</v>
+        <v>33817</v>
       </c>
       <c r="E278" t="s">
         <v>71</v>
@@ -5749,13 +5795,13 @@
         <v>164</v>
       </c>
       <c r="B279" s="2">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C279" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D279" s="3">
-        <v>36008</v>
+        <v>33848</v>
       </c>
       <c r="E279" t="s">
         <v>71</v>
@@ -5766,13 +5812,13 @@
         <v>164</v>
       </c>
       <c r="B280" s="2">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C280" t="s">
-        <v>169</v>
-      </c>
-      <c r="D280" s="3">
-        <v>36495</v>
+        <v>222</v>
+      </c>
+      <c r="D280" t="s">
+        <v>181</v>
       </c>
       <c r="E280" t="s">
         <v>71</v>
@@ -5783,16 +5829,16 @@
         <v>164</v>
       </c>
       <c r="B281" s="2">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C281" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D281" s="3">
-        <v>36526</v>
+        <v>33878</v>
       </c>
       <c r="E281" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -5800,13 +5846,13 @@
         <v>164</v>
       </c>
       <c r="B282" s="2">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C282" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D282" s="3">
-        <v>36557</v>
+        <v>34274</v>
       </c>
       <c r="E282" t="s">
         <v>71</v>
@@ -5817,13 +5863,13 @@
         <v>164</v>
       </c>
       <c r="B283" s="2">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C283" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D283" s="3">
-        <v>36617</v>
+        <v>36008</v>
       </c>
       <c r="E283" t="s">
         <v>71</v>
@@ -5834,13 +5880,13 @@
         <v>164</v>
       </c>
       <c r="B284" s="2">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C284" t="s">
-        <v>169</v>
-      </c>
-      <c r="D284" t="s">
-        <v>183</v>
+        <v>222</v>
+      </c>
+      <c r="D284" s="3">
+        <v>36495</v>
       </c>
       <c r="E284" t="s">
         <v>71</v>
@@ -5851,13 +5897,13 @@
         <v>164</v>
       </c>
       <c r="B285" s="2">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C285" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D285" s="3">
-        <v>36678</v>
+        <v>36526</v>
       </c>
       <c r="E285" t="s">
         <v>75</v>
@@ -5868,13 +5914,13 @@
         <v>164</v>
       </c>
       <c r="B286" s="2">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C286" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D286" s="3">
-        <v>36770</v>
+        <v>36557</v>
       </c>
       <c r="E286" t="s">
         <v>71</v>
@@ -5885,13 +5931,13 @@
         <v>164</v>
       </c>
       <c r="B287" s="2">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C287" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D287" s="3">
-        <v>36800</v>
+        <v>36617</v>
       </c>
       <c r="E287" t="s">
         <v>71</v>
@@ -5902,13 +5948,13 @@
         <v>164</v>
       </c>
       <c r="B288" s="2">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C288" t="s">
-        <v>169</v>
-      </c>
-      <c r="D288" s="3">
-        <v>36831</v>
+        <v>222</v>
+      </c>
+      <c r="D288" t="s">
+        <v>182</v>
       </c>
       <c r="E288" t="s">
         <v>71</v>
@@ -5919,13 +5965,13 @@
         <v>164</v>
       </c>
       <c r="B289" s="2">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C289" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D289" s="3">
-        <v>36861</v>
+        <v>36678</v>
       </c>
       <c r="E289" t="s">
         <v>75</v>
@@ -5936,13 +5982,13 @@
         <v>164</v>
       </c>
       <c r="B290" s="2">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C290" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D290" s="3">
-        <v>36892</v>
+        <v>36770</v>
       </c>
       <c r="E290" t="s">
         <v>71</v>
@@ -5953,13 +5999,13 @@
         <v>164</v>
       </c>
       <c r="B291" s="2">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C291" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D291" s="3">
-        <v>36923</v>
+        <v>36800</v>
       </c>
       <c r="E291" t="s">
         <v>71</v>
@@ -5970,13 +6016,13 @@
         <v>164</v>
       </c>
       <c r="B292" s="2">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C292" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D292" s="3">
-        <v>36951</v>
+        <v>36831</v>
       </c>
       <c r="E292" t="s">
         <v>71</v>
@@ -5987,16 +6033,16 @@
         <v>164</v>
       </c>
       <c r="B293" s="2">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C293" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D293" s="3">
-        <v>36982</v>
+        <v>36861</v>
       </c>
       <c r="E293" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -6004,13 +6050,13 @@
         <v>164</v>
       </c>
       <c r="B294" s="2">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C294" t="s">
-        <v>169</v>
-      </c>
-      <c r="D294" t="s">
-        <v>184</v>
+        <v>222</v>
+      </c>
+      <c r="D294" s="3">
+        <v>36892</v>
       </c>
       <c r="E294" t="s">
         <v>71</v>
@@ -6021,13 +6067,13 @@
         <v>164</v>
       </c>
       <c r="B295" s="2">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C295" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D295" s="3">
-        <v>37043</v>
+        <v>36923</v>
       </c>
       <c r="E295" t="s">
         <v>71</v>
@@ -6038,16 +6084,16 @@
         <v>164</v>
       </c>
       <c r="B296" s="2">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C296" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D296" s="3">
-        <v>37073</v>
+        <v>36951</v>
       </c>
       <c r="E296" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -6055,13 +6101,13 @@
         <v>164</v>
       </c>
       <c r="B297" s="2">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C297" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D297" s="3">
-        <v>37104</v>
+        <v>36982</v>
       </c>
       <c r="E297" t="s">
         <v>71</v>
@@ -6072,13 +6118,13 @@
         <v>164</v>
       </c>
       <c r="B298" s="2">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C298" t="s">
-        <v>169</v>
-      </c>
-      <c r="D298" s="3">
-        <v>37135</v>
+        <v>222</v>
+      </c>
+      <c r="D298" t="s">
+        <v>183</v>
       </c>
       <c r="E298" t="s">
         <v>71</v>
@@ -6089,16 +6135,16 @@
         <v>164</v>
       </c>
       <c r="B299" s="2">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C299" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D299" s="3">
-        <v>37165</v>
+        <v>37043</v>
       </c>
       <c r="E299" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -6106,16 +6152,16 @@
         <v>164</v>
       </c>
       <c r="B300" s="2">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C300" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D300" s="3">
-        <v>37196</v>
+        <v>37073</v>
       </c>
       <c r="E300" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -6123,16 +6169,16 @@
         <v>164</v>
       </c>
       <c r="B301" s="2">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C301" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D301" s="3">
-        <v>37226</v>
+        <v>37104</v>
       </c>
       <c r="E301" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -6140,13 +6186,13 @@
         <v>164</v>
       </c>
       <c r="B302" s="2">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C302" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D302" s="3">
-        <v>37288</v>
+        <v>37135</v>
       </c>
       <c r="E302" t="s">
         <v>71</v>
@@ -6157,16 +6203,16 @@
         <v>164</v>
       </c>
       <c r="B303" s="2">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C303" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D303" s="3">
-        <v>37316</v>
+        <v>37165</v>
       </c>
       <c r="E303" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -6174,13 +6220,13 @@
         <v>164</v>
       </c>
       <c r="B304" s="2">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C304" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D304" s="3">
-        <v>37712</v>
+        <v>37196</v>
       </c>
       <c r="E304" t="s">
         <v>71</v>
@@ -6191,16 +6237,16 @@
         <v>164</v>
       </c>
       <c r="B305" s="2">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C305" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D305" s="3">
-        <v>38384</v>
+        <v>37226</v>
       </c>
       <c r="E305" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
@@ -6208,13 +6254,13 @@
         <v>164</v>
       </c>
       <c r="B306" s="2">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C306" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D306" s="3">
-        <v>38412</v>
+        <v>37288</v>
       </c>
       <c r="E306" t="s">
         <v>71</v>
@@ -6225,13 +6271,13 @@
         <v>164</v>
       </c>
       <c r="B307" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C307" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D307" s="3">
-        <v>38443</v>
+        <v>37316</v>
       </c>
       <c r="E307" t="s">
         <v>71</v>
@@ -6242,13 +6288,13 @@
         <v>164</v>
       </c>
       <c r="B308" s="2">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C308" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D308" s="3">
-        <v>39173</v>
+        <v>37712</v>
       </c>
       <c r="E308" t="s">
         <v>71</v>
@@ -6259,16 +6305,16 @@
         <v>164</v>
       </c>
       <c r="B309" s="2">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C309" t="s">
-        <v>185</v>
-      </c>
-      <c r="D309" t="s">
-        <v>186</v>
+        <v>222</v>
+      </c>
+      <c r="D309" s="3">
+        <v>38384</v>
       </c>
       <c r="E309" t="s">
-        <v>188</v>
+        <v>71</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
@@ -6276,16 +6322,16 @@
         <v>164</v>
       </c>
       <c r="B310" s="2">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C310" t="s">
-        <v>185</v>
-      </c>
-      <c r="D310" t="s">
-        <v>187</v>
+        <v>222</v>
+      </c>
+      <c r="D310" s="3">
+        <v>38412</v>
       </c>
       <c r="E310" t="s">
-        <v>189</v>
+        <v>71</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -6293,16 +6339,16 @@
         <v>164</v>
       </c>
       <c r="B311" s="2">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C311" t="s">
-        <v>185</v>
+        <v>222</v>
       </c>
       <c r="D311" s="3">
-        <v>33055</v>
+        <v>38443</v>
       </c>
       <c r="E311" t="s">
-        <v>190</v>
+        <v>71</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
@@ -6310,16 +6356,16 @@
         <v>164</v>
       </c>
       <c r="B312" s="2">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C312" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="D312" s="3">
-        <v>32509</v>
+        <v>39173</v>
       </c>
       <c r="E312" t="s">
-        <v>192</v>
+        <v>71</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -6327,16 +6373,16 @@
         <v>164</v>
       </c>
       <c r="B313" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C313" t="s">
-        <v>191</v>
-      </c>
-      <c r="D313" s="3">
-        <v>32540</v>
+        <v>184</v>
+      </c>
+      <c r="D313" t="s">
+        <v>185</v>
       </c>
       <c r="E313" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
@@ -6344,16 +6390,16 @@
         <v>164</v>
       </c>
       <c r="B314" s="2">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C314" t="s">
-        <v>191</v>
-      </c>
-      <c r="D314" s="3">
-        <v>32568</v>
+        <v>184</v>
+      </c>
+      <c r="D314" t="s">
+        <v>186</v>
       </c>
       <c r="E314" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
@@ -6361,16 +6407,16 @@
         <v>164</v>
       </c>
       <c r="B315" s="2">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C315" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D315" s="3">
-        <v>32599</v>
+        <v>33055</v>
       </c>
       <c r="E315" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
@@ -6378,16 +6424,16 @@
         <v>164</v>
       </c>
       <c r="B316" s="2">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C316" t="s">
+        <v>190</v>
+      </c>
+      <c r="D316" s="3">
+        <v>32509</v>
+      </c>
+      <c r="E316" t="s">
         <v>191</v>
-      </c>
-      <c r="D316" s="3">
-        <v>32629</v>
-      </c>
-      <c r="E316" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
@@ -6395,16 +6441,16 @@
         <v>164</v>
       </c>
       <c r="B317" s="2">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C317" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D317" s="3">
-        <v>32660</v>
+        <v>32540</v>
       </c>
       <c r="E317" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
@@ -6412,16 +6458,16 @@
         <v>164</v>
       </c>
       <c r="B318" s="2">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C318" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D318" s="3">
-        <v>32690</v>
+        <v>32568</v>
       </c>
       <c r="E318" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
@@ -6429,16 +6475,16 @@
         <v>164</v>
       </c>
       <c r="B319" s="2">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C319" t="s">
-        <v>191</v>
-      </c>
-      <c r="D319" t="s">
-        <v>175</v>
+        <v>190</v>
+      </c>
+      <c r="D319" s="3">
+        <v>32599</v>
       </c>
       <c r="E319" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
@@ -6446,16 +6492,16 @@
         <v>164</v>
       </c>
       <c r="B320" s="2">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C320" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D320" s="3">
-        <v>32782</v>
+        <v>32629</v>
       </c>
       <c r="E320" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
@@ -6463,16 +6509,16 @@
         <v>164</v>
       </c>
       <c r="B321" s="2">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C321" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D321" s="3">
-        <v>32813</v>
+        <v>32660</v>
       </c>
       <c r="E321" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
@@ -6480,16 +6526,16 @@
         <v>164</v>
       </c>
       <c r="B322" s="2">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C322" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D322" s="3">
-        <v>32874</v>
+        <v>32690</v>
       </c>
       <c r="E322" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
@@ -6497,16 +6543,16 @@
         <v>164</v>
       </c>
       <c r="B323" s="2">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C323" t="s">
-        <v>191</v>
-      </c>
-      <c r="D323" s="3">
-        <v>32905</v>
+        <v>190</v>
+      </c>
+      <c r="D323" t="s">
+        <v>174</v>
       </c>
       <c r="E323" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
@@ -6514,16 +6560,16 @@
         <v>164</v>
       </c>
       <c r="B324" s="2">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C324" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D324" s="3">
-        <v>32933</v>
+        <v>32782</v>
       </c>
       <c r="E324" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
@@ -6531,16 +6577,16 @@
         <v>164</v>
       </c>
       <c r="B325" s="2">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C325" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D325" s="3">
-        <v>32964</v>
+        <v>32813</v>
       </c>
       <c r="E325" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -6548,16 +6594,16 @@
         <v>164</v>
       </c>
       <c r="B326" s="2">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C326" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D326" s="3">
-        <v>32994</v>
+        <v>32874</v>
       </c>
       <c r="E326" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
@@ -6565,16 +6611,16 @@
         <v>164</v>
       </c>
       <c r="B327" s="2">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C327" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D327" s="3">
-        <v>33025</v>
+        <v>32905</v>
       </c>
       <c r="E327" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
@@ -6582,16 +6628,16 @@
         <v>164</v>
       </c>
       <c r="B328" s="2">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C328" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D328" s="3">
-        <v>33055</v>
+        <v>32933</v>
       </c>
       <c r="E328" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -6599,16 +6645,16 @@
         <v>164</v>
       </c>
       <c r="B329" s="2">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C329" t="s">
-        <v>191</v>
-      </c>
-      <c r="D329" t="s">
-        <v>206</v>
+        <v>190</v>
+      </c>
+      <c r="D329" s="3">
+        <v>32964</v>
       </c>
       <c r="E329" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
@@ -6616,16 +6662,16 @@
         <v>164</v>
       </c>
       <c r="B330" s="2">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C330" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D330" s="3">
-        <v>33147</v>
+        <v>32994</v>
       </c>
       <c r="E330" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
@@ -6633,16 +6679,16 @@
         <v>164</v>
       </c>
       <c r="B331" s="2">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C331" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D331" s="3">
-        <v>33178</v>
+        <v>33025</v>
       </c>
       <c r="E331" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -6650,16 +6696,16 @@
         <v>164</v>
       </c>
       <c r="B332" s="2">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C332" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D332" s="3">
-        <v>33208</v>
+        <v>33055</v>
       </c>
       <c r="E332" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -6667,16 +6713,132 @@
         <v>164</v>
       </c>
       <c r="B333" s="2">
+        <v>94</v>
+      </c>
+      <c r="C333" t="s">
+        <v>190</v>
+      </c>
+      <c r="D333" t="s">
+        <v>205</v>
+      </c>
+      <c r="E333" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A334" s="1">
+        <v>164</v>
+      </c>
+      <c r="B334" s="2">
+        <v>95</v>
+      </c>
+      <c r="C334" t="s">
+        <v>190</v>
+      </c>
+      <c r="D334" s="3">
+        <v>33147</v>
+      </c>
+      <c r="E334" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A335" s="1">
+        <v>164</v>
+      </c>
+      <c r="B335" s="2">
+        <v>96</v>
+      </c>
+      <c r="C335" t="s">
+        <v>190</v>
+      </c>
+      <c r="D335" s="3">
+        <v>33178</v>
+      </c>
+      <c r="E335" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A336" s="1">
+        <v>164</v>
+      </c>
+      <c r="B336" s="2">
+        <v>97</v>
+      </c>
+      <c r="C336" t="s">
+        <v>190</v>
+      </c>
+      <c r="D336" s="3">
+        <v>33208</v>
+      </c>
+      <c r="E336" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A337" s="1">
+        <v>164</v>
+      </c>
+      <c r="B337" s="2">
         <v>98</v>
       </c>
-      <c r="C333" t="s">
-        <v>205</v>
-      </c>
-      <c r="D333" t="s">
-        <v>207</v>
-      </c>
-      <c r="E333" t="s">
-        <v>71</v>
+      <c r="C337" t="s">
+        <v>204</v>
+      </c>
+      <c r="D337" t="s">
+        <v>206</v>
+      </c>
+      <c r="E337" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A338" s="1">
+        <v>164</v>
+      </c>
+      <c r="B338" s="2">
+        <v>99</v>
+      </c>
+      <c r="C338" t="s">
+        <v>215</v>
+      </c>
+      <c r="D338" s="6">
+        <v>1993</v>
+      </c>
+      <c r="E338" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A339" s="1">
+        <v>164</v>
+      </c>
+      <c r="B339" s="2">
+        <v>100</v>
+      </c>
+      <c r="C339" t="s">
+        <v>217</v>
+      </c>
+      <c r="D339" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E339" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A340" s="1">
+        <v>164</v>
+      </c>
+      <c r="B340" s="2">
+        <v>101</v>
+      </c>
+      <c r="C340" t="s">
+        <v>220</v>
+      </c>
+      <c r="D340" s="6" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>